<commit_message>
Apex treatment to insert Lead records
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28502"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apope/Desktop/Manage Data Successfully/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remil\3D Objects\ExcelToRecords\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2218E97-7640-4C96-997D-2A4A82AD7264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leads" sheetId="1" r:id="rId1"/>
@@ -296,9 +297,6 @@
     <t>RTP</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>Benavides</t>
   </si>
   <si>
@@ -821,22 +819,25 @@
     <t>Open</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
     <t>Address Line 1</t>
   </si>
   <si>
     <t>Postal Code</t>
   </si>
   <si>
-    <t>Last Name</t>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1320,54 +1321,57 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1659,41 +1663,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="34.1640625" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.1796875" customWidth="1"/>
+    <col min="6" max="6" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="7.36328125" customWidth="1"/>
+    <col min="12" max="12" width="13.6328125" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1702,51 +1706,51 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>85</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G2" t="s">
         <v>57</v>
@@ -1764,19 +1768,19 @@
         <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1784,25 +1788,25 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" t="s">
         <v>120</v>
       </c>
-      <c r="F3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H3" t="s">
-        <v>121</v>
-      </c>
       <c r="I3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J3">
         <v>27718</v>
@@ -1811,19 +1815,19 @@
         <v>5</v>
       </c>
       <c r="L3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1831,25 +1835,25 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H4" t="s">
         <v>87</v>
       </c>
       <c r="I4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J4">
         <v>27709</v>
@@ -1858,19 +1862,19 @@
         <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1878,25 +1882,25 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J5">
         <v>27715</v>
@@ -1905,19 +1909,19 @@
         <v>5</v>
       </c>
       <c r="L5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1925,25 +1929,25 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H6" t="s">
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J6">
         <v>94108</v>
@@ -1952,19 +1956,19 @@
         <v>5</v>
       </c>
       <c r="L6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O6" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1972,19 +1976,19 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H7" t="s">
         <v>33</v>
@@ -1999,19 +2003,19 @@
         <v>5</v>
       </c>
       <c r="L7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -2019,22 +2023,22 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D8" t="s">
         <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I8" t="s">
         <v>2</v>
@@ -2046,39 +2050,39 @@
         <v>5</v>
       </c>
       <c r="L8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O8" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H9" t="s">
         <v>4</v>
@@ -2093,19 +2097,19 @@
         <v>5</v>
       </c>
       <c r="L9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -2113,25 +2117,25 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D10" t="s">
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J10">
         <v>27714</v>
@@ -2140,45 +2144,45 @@
         <v>5</v>
       </c>
       <c r="L10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O10" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G11" t="s">
         <v>43</v>
       </c>
       <c r="H11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J11">
         <v>27721</v>
@@ -2187,19 +2191,19 @@
         <v>5</v>
       </c>
       <c r="L11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O11" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2207,19 +2211,19 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H12" t="s">
         <v>4</v>
@@ -2234,19 +2238,19 @@
         <v>5</v>
       </c>
       <c r="L12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O12" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2254,19 +2258,19 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H13" t="s">
         <v>4</v>
@@ -2281,19 +2285,19 @@
         <v>5</v>
       </c>
       <c r="L13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2301,25 +2305,25 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J14">
         <v>27719</v>
@@ -2328,19 +2332,19 @@
         <v>5</v>
       </c>
       <c r="L14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O14" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2348,25 +2352,25 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H15" t="s">
         <v>33</v>
       </c>
       <c r="I15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J15">
         <v>94603</v>
@@ -2375,19 +2379,19 @@
         <v>5</v>
       </c>
       <c r="L15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -2395,16 +2399,16 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G16" t="s">
         <v>32</v>
@@ -2422,19 +2426,19 @@
         <v>5</v>
       </c>
       <c r="L16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O16" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2442,25 +2446,25 @@
         <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J17">
         <v>27716</v>
@@ -2469,19 +2473,19 @@
         <v>5</v>
       </c>
       <c r="L17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O17" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2489,19 +2493,19 @@
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H18" t="s">
         <v>4</v>
@@ -2516,19 +2520,19 @@
         <v>5</v>
       </c>
       <c r="L18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O18" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2536,22 +2540,22 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I19" t="s">
         <v>2</v>
@@ -2563,19 +2567,19 @@
         <v>5</v>
       </c>
       <c r="L19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O19" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -2583,25 +2587,25 @@
         <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J20">
         <v>27712</v>
@@ -2610,19 +2614,19 @@
         <v>5</v>
       </c>
       <c r="L20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O20" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2630,25 +2634,25 @@
         <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J21">
         <v>27710</v>
@@ -2657,19 +2661,19 @@
         <v>5</v>
       </c>
       <c r="L21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O21" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2677,25 +2681,25 @@
         <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J22">
         <v>94114</v>
@@ -2704,19 +2708,19 @@
         <v>5</v>
       </c>
       <c r="L22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O22" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -2724,16 +2728,16 @@
         <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D23" t="s">
         <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G23" t="s">
         <v>46</v>
@@ -2751,19 +2755,19 @@
         <v>5</v>
       </c>
       <c r="L23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O23" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -2771,25 +2775,25 @@
         <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D24" t="s">
         <v>83</v>
       </c>
       <c r="E24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J24">
         <v>27711</v>
@@ -2798,19 +2802,19 @@
         <v>5</v>
       </c>
       <c r="L24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O24" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -2818,25 +2822,25 @@
         <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H25" t="s">
         <v>87</v>
       </c>
       <c r="I25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J25">
         <v>27717</v>
@@ -2845,19 +2849,19 @@
         <v>5</v>
       </c>
       <c r="L25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O25" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2865,25 +2869,25 @@
         <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J26">
         <v>27722</v>
@@ -2892,45 +2896,45 @@
         <v>5</v>
       </c>
       <c r="L26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O26" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H27" t="s">
         <v>33</v>
       </c>
       <c r="I27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J27">
         <v>94599</v>
@@ -2939,42 +2943,42 @@
         <v>5</v>
       </c>
       <c r="L27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O27" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I28" t="s">
         <v>2</v>
@@ -2986,19 +2990,19 @@
         <v>5</v>
       </c>
       <c r="L28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O28" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -3006,16 +3010,16 @@
         <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F29" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G29" t="s">
         <v>43</v>
@@ -3024,7 +3028,7 @@
         <v>87</v>
       </c>
       <c r="I29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J29">
         <v>27719</v>
@@ -3033,19 +3037,19 @@
         <v>5</v>
       </c>
       <c r="L29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O29" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -3053,19 +3057,19 @@
         <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H30" t="s">
         <v>33</v>
@@ -3080,19 +3084,19 @@
         <v>5</v>
       </c>
       <c r="L30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O30" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -3100,19 +3104,19 @@
         <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H31" t="s">
         <v>4</v>
@@ -3127,19 +3131,19 @@
         <v>5</v>
       </c>
       <c r="L31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O31" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -3147,19 +3151,19 @@
         <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H32" t="s">
         <v>4</v>
@@ -3174,19 +3178,19 @@
         <v>5</v>
       </c>
       <c r="L32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O32" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -3194,25 +3198,25 @@
         <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H33" t="s">
         <v>87</v>
       </c>
       <c r="I33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J33">
         <v>27720</v>
@@ -3221,39 +3225,39 @@
         <v>5</v>
       </c>
       <c r="L33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O33" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H34" t="s">
         <v>4</v>
@@ -3268,19 +3272,19 @@
         <v>5</v>
       </c>
       <c r="L34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O34" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -3288,25 +3292,25 @@
         <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H35" t="s">
         <v>87</v>
       </c>
       <c r="I35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J35">
         <v>27714</v>
@@ -3315,19 +3319,19 @@
         <v>5</v>
       </c>
       <c r="L35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O35" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -3335,25 +3339,25 @@
         <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D36" t="s">
         <v>83</v>
       </c>
       <c r="E36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J36">
         <v>27715</v>
@@ -3362,19 +3366,19 @@
         <v>5</v>
       </c>
       <c r="L36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O36" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -3382,19 +3386,19 @@
         <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H37" t="s">
         <v>4</v>
@@ -3409,19 +3413,19 @@
         <v>5</v>
       </c>
       <c r="L37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O37" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -3429,19 +3433,19 @@
         <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F38" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H38" t="s">
         <v>33</v>
@@ -3456,19 +3460,19 @@
         <v>5</v>
       </c>
       <c r="L38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O38" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -3476,25 +3480,25 @@
         <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D39" t="s">
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F39" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J39">
         <v>27722</v>
@@ -3503,19 +3507,19 @@
         <v>5</v>
       </c>
       <c r="L39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O39" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -3523,19 +3527,19 @@
         <v>56</v>
       </c>
       <c r="C40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H40" t="s">
         <v>4</v>
@@ -3550,45 +3554,45 @@
         <v>5</v>
       </c>
       <c r="L40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O40" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B41" t="s">
         <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H41" t="s">
         <v>33</v>
       </c>
       <c r="I41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J41">
         <v>94602</v>
@@ -3597,19 +3601,19 @@
         <v>5</v>
       </c>
       <c r="L41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O41" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -3617,25 +3621,25 @@
         <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H42" t="s">
         <v>87</v>
       </c>
       <c r="I42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J42">
         <v>27718</v>
@@ -3644,19 +3648,19 @@
         <v>5</v>
       </c>
       <c r="L42" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O42" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -3664,43 +3668,43 @@
         <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F43" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J43">
         <v>27713</v>
       </c>
       <c r="L43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O43" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -3708,25 +3712,25 @@
         <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F44" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J44">
         <v>27720</v>
@@ -3735,19 +3739,19 @@
         <v>5</v>
       </c>
       <c r="L44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O44" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -3755,19 +3759,19 @@
         <v>84</v>
       </c>
       <c r="C45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H45" t="s">
         <v>4</v>
@@ -3779,20 +3783,20 @@
         <v>94113</v>
       </c>
       <c r="L45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O45" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:P50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P50">
     <sortCondition ref="C2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>